<commit_message>
added opportunity test case
</commit_message>
<xml_diff>
--- a/com.greentrade/testdata/TestScriptdata.xlsx
+++ b/com.greentrade/testdata/TestScriptdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EF529C81-808F-495D-BA08-EAB11CE7987D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D20DCDD2-0C30-4BBC-AB77-B932C4A9B7F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6015" activeTab="1" xr2:uid="{2F26AAE5-8F8F-4C9C-AE4A-DE7F1E083FDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15975" windowHeight="6015" firstSheet="1" activeTab="1" xr2:uid="{2F26AAE5-8F8F-4C9C-AE4A-DE7F1E083FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="quotes" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N18"/>
+  <oleSize ref="A1:M18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>Vendor name</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Opportunity Name</t>
   </si>
   <si>
-    <t>Campaign Source</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -121,10 +118,10 @@
     <t>TC_35</t>
   </si>
   <si>
-    <t>Drop down option</t>
-  </si>
-  <si>
-    <t>campaign name</t>
+    <t>TC_33</t>
+  </si>
+  <si>
+    <t>Create new opportunity</t>
   </si>
 </sst>
 </file>
@@ -544,10 +541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF42A8-C2F3-438B-BFE6-ECF569BD974F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,12 +566,39 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -586,10 +610,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99E82DE-0220-445D-BCF2-F33A07A94C4B}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,12 +634,39 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -626,10 +677,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8511C16-3186-4BCE-AA85-4C0D45260E70}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +688,6 @@
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,22 +700,43 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -678,11 +749,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,8 +770,12 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
@@ -714,7 +790,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,14 +832,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -776,24 +851,16 @@
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +873,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,10 +891,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -840,7 +907,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -849,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +929,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,37 +951,37 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -923,10 +990,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added new test cases along with parallel execution
</commit_message>
<xml_diff>
--- a/com.greentrade/testdata/TestScriptdata.xlsx
+++ b/com.greentrade/testdata/TestScriptdata.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D20DCDD2-0C30-4BBC-AB77-B932C4A9B7F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivek\git\greenTradeRepo\com.greentrade\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA253A0-FEF9-48A0-B895-36C5A7960431}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15975" windowHeight="6015" firstSheet="1" activeTab="1" xr2:uid="{2F26AAE5-8F8F-4C9C-AE4A-DE7F1E083FDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="6015" firstSheet="4" activeTab="8" xr2:uid="{2F26AAE5-8F8F-4C9C-AE4A-DE7F1E083FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,6 @@
     <sheet name="quotes" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="36">
   <si>
     <t>Vendor name</t>
   </si>
@@ -79,12 +83,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Contact Last Name</t>
-  </si>
-  <si>
-    <t>Textile Association</t>
-  </si>
-  <si>
     <t>Create Quotes</t>
   </si>
   <si>
@@ -100,9 +98,6 @@
     <t>Billing Address</t>
   </si>
   <si>
-    <t>Item/Product Name</t>
-  </si>
-  <si>
     <t>Maharashtra</t>
   </si>
   <si>
@@ -122,6 +117,30 @@
   </si>
   <si>
     <t>Create new opportunity</t>
+  </si>
+  <si>
+    <t>TC_34</t>
+  </si>
+  <si>
+    <t>Create new  trouble ticket</t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>Generate new quotation</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>2500000.00</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -159,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -182,15 +201,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF42A8-C2F3-438B-BFE6-ECF569BD974F}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +599,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -593,12 +626,66 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -610,10 +697,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99E82DE-0220-445D-BCF2-F33A07A94C4B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,10 +721,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -661,12 +748,66 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -677,10 +818,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8511C16-3186-4BCE-AA85-4C0D45260E70}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +831,7 @@
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -701,23 +842,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -728,14 +869,41 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -746,10 +914,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34192D53-9470-4305-AB73-84F65F1DABA8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,12 +939,66 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -787,18 +1009,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3584E255-EF7B-4D32-96B5-236F518AC017}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -808,18 +1031,43 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -829,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BF1DBD-AE9D-4704-B8A0-D7009DF080CB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +1089,7 @@
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -852,14 +1100,41 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -870,20 +1145,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD8C727-C4A6-4558-B9BF-DD3FCC701A20}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -893,30 +1166,16 @@
       <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -926,24 +1185,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC945D9-3AB1-43A1-9A9F-90278E2DD897}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -951,61 +1207,46 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J2" s="1">
-        <v>9999</v>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated test script file
</commit_message>
<xml_diff>
--- a/com.greentrade/testdata/TestScriptdata.xlsx
+++ b/com.greentrade/testdata/TestScriptdata.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivek\git\greenTradeRepo\com.greentrade\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA253A0-FEF9-48A0-B895-36C5A7960431}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B6BE5E30-D4DF-4491-85D7-BABDE0FCE7EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="6015" firstSheet="4" activeTab="8" xr2:uid="{2F26AAE5-8F8F-4C9C-AE4A-DE7F1E083FDC}"/>
   </bookViews>
@@ -24,6 +19,7 @@
     <sheet name="quotes" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,10 +133,10 @@
     <t>5000</t>
   </si>
   <si>
-    <t>2500000.00</t>
-  </si>
-  <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>2,500,000.00</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1184,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,10 +1235,10 @@
         <v>33</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>